<commit_message>
Switch to scatter plot with a trend line
</commit_message>
<xml_diff>
--- a/data/prices.xlsx
+++ b/data/prices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Halim/git/prices/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02CFCC2F-D173-6F4A-9B3D-C11852C113D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0016FE60-DA06-F043-9BA3-23519A1418C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19760" yWindow="4260" windowWidth="20380" windowHeight="17440" xr2:uid="{467E520F-A507-C645-AF43-7C8F87D202EE}"/>
+    <workbookView xWindow="24140" yWindow="4480" windowWidth="20380" windowHeight="17440" xr2:uid="{467E520F-A507-C645-AF43-7C8F87D202EE}"/>
   </bookViews>
   <sheets>
     <sheet name="PRICES" sheetId="1" r:id="rId1"/>
@@ -515,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0EADCD2-29C8-CC4D-96D3-61A0DB46784B}">
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1124,6 +1124,56 @@
       </c>
       <c r="P12">
         <v>42.33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>45633</v>
+      </c>
+      <c r="B13">
+        <v>22.2</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>2.5</v>
+      </c>
+      <c r="E13">
+        <v>11</v>
+      </c>
+      <c r="F13">
+        <v>4.2</v>
+      </c>
+      <c r="G13">
+        <v>5.7</v>
+      </c>
+      <c r="H13">
+        <v>1.8</v>
+      </c>
+      <c r="I13">
+        <v>1.64</v>
+      </c>
+      <c r="J13">
+        <v>54.95</v>
+      </c>
+      <c r="K13">
+        <v>23.95</v>
+      </c>
+      <c r="L13">
+        <v>419.95</v>
+      </c>
+      <c r="M13">
+        <v>45</v>
+      </c>
+      <c r="N13">
+        <v>104.95</v>
+      </c>
+      <c r="O13">
+        <v>67.5</v>
+      </c>
+      <c r="P13">
+        <v>42.12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refresh after 2 March 2025
</commit_message>
<xml_diff>
--- a/data/prices.xlsx
+++ b/data/prices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Halim/git/prices/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79E0F13-820A-9F43-B0F4-2F0434BE3357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2CB900A-5E3F-A24B-9361-693895084A95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24140" yWindow="4480" windowWidth="20380" windowHeight="17440" xr2:uid="{467E520F-A507-C645-AF43-7C8F87D202EE}"/>
   </bookViews>
@@ -90,9 +90,6 @@
     <t>Bananas (local product in Turkey, Coles default in Australia)</t>
   </si>
   <si>
-    <t>Brown Onions</t>
-  </si>
-  <si>
     <t>Beef Mince (Migros Dana in Turkey, Coles Regular mince in Australia)</t>
   </si>
   <si>
@@ -124,6 +121,9 @@
   </si>
   <si>
     <t>Eggs (Migros orta boy 15-pack in Turkey, Coles free range 12-pack 600g in Australia)</t>
+  </si>
+  <si>
+    <t>Brown Onions (Loose)</t>
   </si>
 </sst>
 </file>
@@ -515,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0EADCD2-29C8-CC4D-96D3-61A0DB46784B}">
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1324,6 +1324,156 @@
       </c>
       <c r="P16">
         <v>45.32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>45691</v>
+      </c>
+      <c r="B17">
+        <v>22.09</v>
+      </c>
+      <c r="C17">
+        <v>2.5</v>
+      </c>
+      <c r="D17">
+        <v>3.6</v>
+      </c>
+      <c r="E17">
+        <v>9</v>
+      </c>
+      <c r="F17">
+        <v>4.2</v>
+      </c>
+      <c r="G17">
+        <v>5.7</v>
+      </c>
+      <c r="H17">
+        <v>1.8</v>
+      </c>
+      <c r="I17">
+        <v>1.659</v>
+      </c>
+      <c r="J17">
+        <v>75.95</v>
+      </c>
+      <c r="K17">
+        <v>14.95</v>
+      </c>
+      <c r="L17">
+        <v>499.95</v>
+      </c>
+      <c r="M17">
+        <v>49.95</v>
+      </c>
+      <c r="N17">
+        <v>109.95</v>
+      </c>
+      <c r="O17">
+        <v>67.5</v>
+      </c>
+      <c r="P17">
+        <v>46.31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>45704</v>
+      </c>
+      <c r="B18">
+        <v>23.02</v>
+      </c>
+      <c r="C18">
+        <v>4.5</v>
+      </c>
+      <c r="D18">
+        <v>3.9</v>
+      </c>
+      <c r="E18">
+        <v>9</v>
+      </c>
+      <c r="F18">
+        <v>4.2</v>
+      </c>
+      <c r="G18">
+        <v>5.7</v>
+      </c>
+      <c r="H18">
+        <v>1.8</v>
+      </c>
+      <c r="I18">
+        <v>1.6990000000000001</v>
+      </c>
+      <c r="J18">
+        <v>75.95</v>
+      </c>
+      <c r="K18">
+        <v>16.95</v>
+      </c>
+      <c r="L18">
+        <v>469.95</v>
+      </c>
+      <c r="M18">
+        <v>49.95</v>
+      </c>
+      <c r="N18">
+        <v>124.95</v>
+      </c>
+      <c r="O18">
+        <v>71.95</v>
+      </c>
+      <c r="P18">
+        <v>46.44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>45718</v>
+      </c>
+      <c r="B19">
+        <v>22.65</v>
+      </c>
+      <c r="C19">
+        <v>4.5</v>
+      </c>
+      <c r="D19">
+        <v>2.5</v>
+      </c>
+      <c r="E19">
+        <v>11</v>
+      </c>
+      <c r="F19">
+        <v>4.2</v>
+      </c>
+      <c r="G19">
+        <v>5.7</v>
+      </c>
+      <c r="H19">
+        <v>1.8</v>
+      </c>
+      <c r="I19">
+        <v>1.9790000000000001</v>
+      </c>
+      <c r="J19">
+        <v>87.95</v>
+      </c>
+      <c r="K19">
+        <v>18.95</v>
+      </c>
+      <c r="L19">
+        <v>579.95000000000005</v>
+      </c>
+      <c r="M19">
+        <v>49.95</v>
+      </c>
+      <c r="N19">
+        <v>134.94999999999999</v>
+      </c>
+      <c r="O19">
+        <v>71.95</v>
+      </c>
+      <c r="P19">
+        <v>46.43</v>
       </c>
     </row>
   </sheetData>
@@ -1346,12 +1496,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1361,48 +1511,48 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
After making x-axis three-tick axis
</commit_message>
<xml_diff>
--- a/data/prices.xlsx
+++ b/data/prices.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Halim/git/prices/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D119AFE7-4C57-A84A-8EFE-7C1089872E61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C69B9D6-2133-F24B-845C-EA8767CBBEFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24140" yWindow="4480" windowWidth="20380" windowHeight="17440" xr2:uid="{467E520F-A507-C645-AF43-7C8F87D202EE}"/>
+    <workbookView xWindow="20580" yWindow="4020" windowWidth="20380" windowHeight="17440" xr2:uid="{467E520F-A507-C645-AF43-7C8F87D202EE}"/>
   </bookViews>
   <sheets>
     <sheet name="PRICES" sheetId="1" r:id="rId1"/>
@@ -515,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0EADCD2-29C8-CC4D-96D3-61A0DB46784B}">
-  <dimension ref="A1:P20"/>
+  <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+      <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1524,6 +1524,106 @@
       </c>
       <c r="P20">
         <v>45.23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>45745</v>
+      </c>
+      <c r="B21">
+        <v>23.88</v>
+      </c>
+      <c r="C21">
+        <v>4.5</v>
+      </c>
+      <c r="D21">
+        <v>2.5</v>
+      </c>
+      <c r="E21">
+        <v>11</v>
+      </c>
+      <c r="F21">
+        <v>4.2</v>
+      </c>
+      <c r="G21">
+        <v>5.7</v>
+      </c>
+      <c r="H21">
+        <v>1.8</v>
+      </c>
+      <c r="I21">
+        <v>1.7949999999999999</v>
+      </c>
+      <c r="J21">
+        <v>89.95</v>
+      </c>
+      <c r="K21">
+        <v>24.95</v>
+      </c>
+      <c r="L21">
+        <v>589.95000000000005</v>
+      </c>
+      <c r="M21">
+        <v>49.95</v>
+      </c>
+      <c r="N21">
+        <v>134.94999999999999</v>
+      </c>
+      <c r="O21">
+        <v>71.95</v>
+      </c>
+      <c r="P21">
+        <v>46.72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>45759</v>
+      </c>
+      <c r="B22">
+        <v>23.92</v>
+      </c>
+      <c r="C22">
+        <v>4.5</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="E22">
+        <v>11</v>
+      </c>
+      <c r="F22">
+        <v>4.2</v>
+      </c>
+      <c r="G22">
+        <v>6.2</v>
+      </c>
+      <c r="H22">
+        <v>1.8</v>
+      </c>
+      <c r="I22">
+        <v>1.6990000000000001</v>
+      </c>
+      <c r="J22">
+        <v>95.95</v>
+      </c>
+      <c r="K22">
+        <v>16.95</v>
+      </c>
+      <c r="L22">
+        <v>589.95000000000005</v>
+      </c>
+      <c r="M22">
+        <v>49.95</v>
+      </c>
+      <c r="N22">
+        <v>154.94999999999999</v>
+      </c>
+      <c r="O22">
+        <v>74.95</v>
+      </c>
+      <c r="P22">
+        <v>44.18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AFter 8 July post
</commit_message>
<xml_diff>
--- a/data/prices.xlsx
+++ b/data/prices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Halim/git/prices/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C2A107-6EC4-1B45-86B4-68DE2588EDDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16DC0C7F-46A7-2C41-A8C9-507BCC779B01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23140" yWindow="4140" windowWidth="20380" windowHeight="17440" xr2:uid="{467E520F-A507-C645-AF43-7C8F87D202EE}"/>
   </bookViews>
@@ -515,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0EADCD2-29C8-CC4D-96D3-61A0DB46784B}">
-  <dimension ref="A1:P26"/>
+  <dimension ref="A1:P28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+      <selection activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1824,6 +1824,106 @@
       </c>
       <c r="P26">
         <v>46.92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>45831</v>
+      </c>
+      <c r="B27">
+        <v>25.36</v>
+      </c>
+      <c r="C27">
+        <v>4.5</v>
+      </c>
+      <c r="D27">
+        <v>2.5</v>
+      </c>
+      <c r="E27">
+        <v>12</v>
+      </c>
+      <c r="F27">
+        <v>4.5</v>
+      </c>
+      <c r="G27">
+        <v>6.2</v>
+      </c>
+      <c r="H27">
+        <v>1.8</v>
+      </c>
+      <c r="I27">
+        <v>1.599</v>
+      </c>
+      <c r="J27">
+        <v>79.95</v>
+      </c>
+      <c r="K27">
+        <v>11.95</v>
+      </c>
+      <c r="L27">
+        <v>549.9</v>
+      </c>
+      <c r="M27">
+        <v>49.95</v>
+      </c>
+      <c r="N27">
+        <v>154.94999999999999</v>
+      </c>
+      <c r="O27">
+        <v>64.95</v>
+      </c>
+      <c r="P27">
+        <v>51.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>45846</v>
+      </c>
+      <c r="B28">
+        <v>26.17</v>
+      </c>
+      <c r="C28">
+        <v>4.5</v>
+      </c>
+      <c r="D28">
+        <v>2.5</v>
+      </c>
+      <c r="E28">
+        <v>12</v>
+      </c>
+      <c r="F28">
+        <v>4.5</v>
+      </c>
+      <c r="G28">
+        <v>6.2</v>
+      </c>
+      <c r="H28">
+        <v>1.8</v>
+      </c>
+      <c r="I28">
+        <v>1.897</v>
+      </c>
+      <c r="J28">
+        <v>119.95</v>
+      </c>
+      <c r="K28">
+        <v>11.95</v>
+      </c>
+      <c r="L28">
+        <v>599.95000000000005</v>
+      </c>
+      <c r="M28">
+        <v>49.95</v>
+      </c>
+      <c r="N28">
+        <v>154.94999999999999</v>
+      </c>
+      <c r="O28">
+        <v>76.95</v>
+      </c>
+      <c r="P28">
+        <v>51.21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>